<commit_message>
Actualizacion de la lista de requerimentos
Se anoto el progreso que se ha hecho a la lista de requerimientos.
</commit_message>
<xml_diff>
--- a/FullStack Avance del Proyecto.xlsx
+++ b/FullStack Avance del Proyecto.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28521"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28528"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03081F1D-C8F5-4A35-9F92-DE37C6102DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9260DDC2-BF5B-4F36-942F-E9F53B143177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -60,21 +60,21 @@
     <t>Documentar el proyecto</t>
   </si>
   <si>
+    <t>Documentar al equipo</t>
+  </si>
+  <si>
+    <t>3-Lead</t>
+  </si>
+  <si>
+    <t>Seguimiento de tareas</t>
+  </si>
+  <si>
+    <t>Documentar todas las tareas completadas</t>
+  </si>
+  <si>
     <t>Incompleta</t>
   </si>
   <si>
-    <t>Documentar al equipo</t>
-  </si>
-  <si>
-    <t>3-Lead</t>
-  </si>
-  <si>
-    <t>Seguimiento de tareas</t>
-  </si>
-  <si>
-    <t>Documentar todas las tareas completadas</t>
-  </si>
-  <si>
     <t>4-Lead</t>
   </si>
   <si>
@@ -108,10 +108,10 @@
     <t>Elegir la basa de datos (MongoDB, MySQL, o PostgreSQL</t>
   </si>
   <si>
-    <t>Instalar dependencias requeridas</t>
-  </si>
-  <si>
-    <t>Configurar proyecto con variables de entorno usando dotenv</t>
+    <t>Desarrollo en HTML</t>
+  </si>
+  <si>
+    <t>Desarrollo en JS</t>
   </si>
   <si>
     <t>Usa IA para consultar un ejemplo de configuracion de variables de entorno utilizando dotenv para almacenar credenciales y claves sensibles</t>
@@ -210,7 +210,7 @@
     <t>Explicacion</t>
   </si>
   <si>
-    <t>Tomar un PR y poner la captura de pantalla explicando como funciona y cual fue el procesos que se sigio para checar que esta bien</t>
+    <t>Tomar un PR y poner la captura de pantalla explicando como funciona y cual fue el proceso que se sigio para checar que esta bien</t>
   </si>
   <si>
     <t>Mostrar colaboradores</t>
@@ -286,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,6 +326,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -418,6 +424,13 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E53"/>
+  <dimension ref="B2:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -853,30 +866,30 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>9</v>
+      <c r="E4" s="20" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:5">
       <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="17" t="s">
         <v>9</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:5">
@@ -890,7 +903,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -898,7 +911,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:5">
@@ -912,7 +925,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:5">
@@ -940,7 +953,7 @@
         <v>23</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:5">
@@ -949,31 +962,31 @@
         <v>24</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>9</v>
+      <c r="E17" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="D18" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>9</v>
+      <c r="E18" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="29.25">
       <c r="D19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>9</v>
+      <c r="E19" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:5">
@@ -986,40 +999,40 @@
       <c r="D20" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="17" t="s">
-        <v>9</v>
+      <c r="E20" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="D21" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>9</v>
+      <c r="E21" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="13.5" customHeight="1">
       <c r="D22" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="17" t="s">
-        <v>9</v>
+      <c r="E22" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:5">
       <c r="D23" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>9</v>
+      <c r="E23" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="2:5">
       <c r="D24" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>9</v>
+      <c r="E24" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="2:5">
@@ -1046,8 +1059,8 @@
       <c r="D27" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>9</v>
+      <c r="E27" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="2:5">
@@ -1056,8 +1069,8 @@
       <c r="D28" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="19" t="s">
-        <v>9</v>
+      <c r="E28" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="29.25">
@@ -1066,8 +1079,8 @@
       <c r="D29" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="19" t="s">
-        <v>9</v>
+      <c r="E29" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="2:5">
@@ -1080,8 +1093,8 @@
       <c r="D30" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="19" t="s">
-        <v>9</v>
+      <c r="E30" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="2:5">
@@ -1094,8 +1107,8 @@
       <c r="D31" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="19" t="s">
-        <v>9</v>
+      <c r="E31" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="2:5">
@@ -1108,8 +1121,8 @@
       <c r="D32" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E32" s="19" t="s">
-        <v>9</v>
+      <c r="E32" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="2:5">
@@ -1118,8 +1131,8 @@
       <c r="D33" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="19" t="s">
-        <v>9</v>
+      <c r="E33" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="2:5">
@@ -1156,8 +1169,8 @@
       <c r="D37" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E37" s="19" t="s">
-        <v>9</v>
+      <c r="E37" s="21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="2:5">
@@ -1174,146 +1187,122 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="10"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="29.25">
-      <c r="B40" s="5" t="s">
+    <row r="39" spans="2:5" ht="29.25">
+      <c r="B39" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C39" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D39" s="13" t="s">
         <v>59</v>
       </c>
+      <c r="E39" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24" t="s">
+        <v>60</v>
+      </c>
       <c r="E40" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5">
-      <c r="B41" s="10"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="5"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="19" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="10"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="19" t="s">
-        <v>9</v>
+      <c r="B43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" s="10"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>3</v>
+      <c r="B46" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="2:5">
-      <c r="B47" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>63</v>
+      <c r="B47" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="2:5">
-      <c r="B48" s="10"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="13" t="s">
-        <v>64</v>
+      <c r="B48" s="5"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="2:5">
-      <c r="B49" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>67</v>
+      <c r="B49" s="10"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="2:5">
-      <c r="B50" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>70</v>
-      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="8"/>
       <c r="E50" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5">
-      <c r="B51" s="5"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5">
-      <c r="B52" s="10"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E52" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5">
-      <c r="B53" s="5"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="19" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Lead   organizacion del equipo - Actualizacion final de los requerimientos"
</commit_message>
<xml_diff>
--- a/FullStack Avance del Proyecto.xlsx
+++ b/FullStack Avance del Proyecto.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28528"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josue\Desktop\Nexo\Vida y Trabajo\Escuela\Facultad\Tec Milenio\Tercer Semestre (Tecmilenio)\Desarrollo Full Stack\Avance del Proyecto\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B933F809-CCCE-4DC9-A128-DA08E95F449C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9260DDC2-BF5B-4F36-942F-E9F53B143177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -75,6 +70,9 @@
   </si>
   <si>
     <t>Documentar todas las tareas completadas</t>
+  </si>
+  <si>
+    <t>Incompleta</t>
   </si>
   <si>
     <t>4-Lead</t>
@@ -258,7 +256,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +314,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD45324"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE30E0E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -389,43 +393,44 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,11 +814,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="35.5703125" customWidth="1"/>
@@ -821,7 +826,7 @@
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -835,7 +840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5">
       <c r="B3" t="str">
         <f>TEXT(ROW() - ROW(Tabla1[[#Headers],[ID]]), "[$-es-ES]0;-0") &amp; "-Lead"</f>
         <v>1-Lead</v>
@@ -846,11 +851,11 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
       <c r="B4" t="str">
         <f>TEXT(ROW() - ROW(Tabla1[[#Headers],[ID]]), "[$-es-ES]0;-0") &amp; "-Lead"</f>
         <v>2-Lead</v>
@@ -861,19 +866,19 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -883,47 +888,47 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:5">
       <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -937,100 +942,100 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5">
       <c r="B15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
       <c r="C16" s="1"/>
       <c r="D16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
       <c r="D17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
       <c r="D18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="29.25">
       <c r="D19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
       <c r="D21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="13.5" customHeight="1">
       <c r="D22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
       <c r="D23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
       <c r="D24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26" s="2" t="s">
         <v>0</v>
       </c>
@@ -1040,97 +1045,97 @@
       <c r="D26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" ht="29.25">
       <c r="B27" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
       <c r="D28" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="29.25">
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="D29" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
       <c r="B30" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
       <c r="B31" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
       <c r="B32" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
       <c r="D33" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
       <c r="B35" s="2" t="s">
         <v>0</v>
       </c>
@@ -1140,73 +1145,73 @@
       <c r="D35" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5">
       <c r="B36" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
       <c r="B37" s="10"/>
       <c r="C37" s="15"/>
       <c r="D37" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
       <c r="B38" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="29.25">
       <c r="B39" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="20"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="22" t="s">
         <v>59</v>
       </c>
+      <c r="E39" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24" t="s">
+        <v>60</v>
+      </c>
       <c r="E40" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
       <c r="B43" s="2" t="s">
         <v>0</v>
       </c>
@@ -1216,88 +1221,88 @@
       <c r="D43" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E43" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5">
       <c r="B44" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
       <c r="B45" s="10"/>
       <c r="C45" s="15"/>
       <c r="D45" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E45" s="23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5">
       <c r="B46" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
       <c r="B47" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5">
       <c r="B48" s="5"/>
       <c r="C48" s="9"/>
       <c r="D48" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E48" s="23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
       <c r="B49" s="10"/>
       <c r="C49" s="15"/>
       <c r="D49" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E49" s="23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
       <c r="B50" s="5"/>
       <c r="C50" s="9"/>
       <c r="D50" s="8"/>
-      <c r="E50" s="23" t="s">
-        <v>6</v>
+      <c r="E50" s="19" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>